<commit_message>
change order diferences of payroll2 - payroll1 to payroll1- payroll2
</commit_message>
<xml_diff>
--- a/compare_payroll_template.xlsx
+++ b/compare_payroll_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Documents\Projetos\Moresco\Java-SCI-ComparePayroll\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C3EB354-B022-425A-A160-B5B3595EA519}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAF35C49-9209-4154-9C73-66E1BC6B2573}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="00.Alerta" sheetId="3" r:id="rId1"/>
@@ -237,10 +237,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -255,7 +255,50 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -563,7 +606,7 @@
   </sheetPr>
   <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
@@ -631,47 +674,47 @@
     <row r="4" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="1"/>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="22"/>
-      <c r="K4" s="22"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
       <c r="L4" s="1"/>
       <c r="M4" s="3"/>
     </row>
     <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="1"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
-      <c r="J5" s="22"/>
-      <c r="K5" s="22"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
       <c r="L5" s="1"/>
       <c r="M5" s="3"/>
     </row>
     <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="1"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22"/>
-      <c r="J6" s="22"/>
-      <c r="K6" s="22"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
       <c r="L6" s="1"/>
       <c r="M6" s="3"/>
     </row>
@@ -693,17 +736,17 @@
     <row r="8" spans="1:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="20"/>
       <c r="B8" s="1"/>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="22"/>
-      <c r="K8" s="22"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
       <c r="L8" s="1"/>
       <c r="M8" s="20"/>
     </row>
@@ -789,15 +832,15 @@
     <row r="4" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="1"/>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
       <c r="J4" s="1"/>
       <c r="K4" s="3"/>
       <c r="L4" s="1"/>
@@ -806,13 +849,13 @@
     <row r="5" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="1"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
       <c r="J5" s="1"/>
       <c r="K5" s="3"/>
       <c r="L5" s="1"/>
@@ -821,13 +864,13 @@
     <row r="6" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="1"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
       <c r="J6" s="1"/>
       <c r="K6" s="3"/>
       <c r="L6" s="1"/>
@@ -945,41 +988,41 @@
     <row r="4" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="1"/>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
       <c r="J4" s="1"/>
       <c r="K4" s="3"/>
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="1"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
       <c r="J5" s="1"/>
       <c r="K5" s="3"/>
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="1"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
       <c r="J6" s="1"/>
       <c r="K6" s="3"/>
     </row>
@@ -1032,8 +1075,8 @@
   </sheetPr>
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1108,8 +1151,8 @@
         <v>1</v>
       </c>
       <c r="I4" s="10">
-        <f>COUNTA(#REF!)</f>
-        <v>1</v>
+        <f>COUNTA(E9:E1000000)</f>
+        <v>0</v>
       </c>
       <c r="J4" s="11"/>
       <c r="K4" s="1"/>
@@ -1127,8 +1170,8 @@
         <v>2</v>
       </c>
       <c r="I5" s="10">
-        <f>COUNTA(#REF!)</f>
-        <v>1</v>
+        <f>COUNTA(I9:I1000000)</f>
+        <v>0</v>
       </c>
       <c r="J5" s="11"/>
       <c r="K5" s="1"/>
@@ -1194,6 +1237,37 @@
   <mergeCells count="1">
     <mergeCell ref="C4:G6"/>
   </mergeCells>
+  <conditionalFormatting sqref="C9:C1048576">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="7">
+      <formula>LEN(TRIM(C9))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D9:D1048576">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="5">
+      <formula>LEN(TRIM(D9))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9:E1048576">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+      <formula>"Diferença"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F9:F1048576">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>"Valor Diferença"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G9:G1048576">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>$F9="Valor Diferença"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H9:H1048576">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$F9="Valor Diferença"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>